<commit_message>
Added SFR leakage output
</commit_message>
<xml_diff>
--- a/data/observations/obs_flow_and_stage.xlsx
+++ b/data/observations/obs_flow_and_stage.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>POINT_X</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>INFLOW</t>
+  </si>
+  <si>
+    <t>GAGE-2</t>
   </si>
 </sst>
 </file>
@@ -372,10 +375,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -473,12 +476,26 @@
         <v>10</v>
       </c>
       <c r="B7">
+        <v>427070.614</v>
+      </c>
+      <c r="C7">
+        <v>6654948.9349999996</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8">
         <v>427030.76</v>
       </c>
-      <c r="C7">
+      <c r="C8">
         <v>6654934.2599999998</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>